<commit_message>
added fxHashmap and compile options for faster programg
</commit_message>
<xml_diff>
--- a/tests/benchmarks.xlsx
+++ b/tests/benchmarks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjeer\OneDrive - Universiteit Utrecht\Desktop\Master thesis\jip\Jip\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0B1664-97D0-4B0B-91C0-133477516A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED749EE8-921C-4A09-B156-C3445B454EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="fibonaci" sheetId="1" r:id="rId1"/>
+    <sheet name="Build configs" sheetId="2" r:id="rId1"/>
+    <sheet name="fibonaci" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>b858cd0</t>
   </si>
@@ -76,6 +77,327 @@
   </si>
   <si>
     <t>229.2223026s</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>Fibonacci program - commit 8c2d859</t>
+  </si>
+  <si>
+    <t>lto = true</t>
+  </si>
+  <si>
+    <t>codegen-units = 1</t>
+  </si>
+  <si>
+    <t>RUSTFLAGS="-C target-cpu=native" cargo build --release</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>release (no extra config)</t>
+  </si>
+  <si>
+    <t>9.1117ms</t>
+  </si>
+  <si>
+    <t>10.5018ms</t>
+  </si>
+  <si>
+    <t>64.9126ms</t>
+  </si>
+  <si>
+    <t>84.916ms</t>
+  </si>
+  <si>
+    <t>109.2766ms</t>
+  </si>
+  <si>
+    <t>280.4703ms</t>
+  </si>
+  <si>
+    <t>307.8501ms</t>
+  </si>
+  <si>
+    <t>497.6233ms</t>
+  </si>
+  <si>
+    <t>1.0445285s</t>
+  </si>
+  <si>
+    <t>1.9787045s</t>
+  </si>
+  <si>
+    <t>3.9539033s</t>
+  </si>
+  <si>
+    <t>4.9832485s</t>
+  </si>
+  <si>
+    <t>8.6718677s</t>
+  </si>
+  <si>
+    <t>28.8492059s</t>
+  </si>
+  <si>
+    <t>38.2159568s</t>
+  </si>
+  <si>
+    <t>69.7549288s</t>
+  </si>
+  <si>
+    <t>7.8656ms</t>
+  </si>
+  <si>
+    <t>7.9665ms</t>
+  </si>
+  <si>
+    <t>48.561ms</t>
+  </si>
+  <si>
+    <t>50.7566ms</t>
+  </si>
+  <si>
+    <t>77.4546ms</t>
+  </si>
+  <si>
+    <t>169.183ms</t>
+  </si>
+  <si>
+    <t>201.5488ms</t>
+  </si>
+  <si>
+    <t>297.9806ms</t>
+  </si>
+  <si>
+    <t>911.9439ms</t>
+  </si>
+  <si>
+    <t>1.5744228s</t>
+  </si>
+  <si>
+    <t>4.4149806s</t>
+  </si>
+  <si>
+    <t>5.1125973s</t>
+  </si>
+  <si>
+    <t>7.9721571s</t>
+  </si>
+  <si>
+    <t>25.4962324s</t>
+  </si>
+  <si>
+    <t>36.2301075s</t>
+  </si>
+  <si>
+    <t>65.823365s</t>
+  </si>
+  <si>
+    <t>debug + rustc_hash</t>
+  </si>
+  <si>
+    <t>33.145ms</t>
+  </si>
+  <si>
+    <t>47.8339ms</t>
+  </si>
+  <si>
+    <t>133.4568ms</t>
+  </si>
+  <si>
+    <t>141.9002ms</t>
+  </si>
+  <si>
+    <t>202.7826ms</t>
+  </si>
+  <si>
+    <t>600.751ms</t>
+  </si>
+  <si>
+    <t>746.227ms</t>
+  </si>
+  <si>
+    <t>966.4747ms</t>
+  </si>
+  <si>
+    <t>2.5170463s</t>
+  </si>
+  <si>
+    <t>3.0177107s</t>
+  </si>
+  <si>
+    <t>6.3129194s</t>
+  </si>
+  <si>
+    <t>11.3568047s</t>
+  </si>
+  <si>
+    <t>17.2293933s</t>
+  </si>
+  <si>
+    <t>38.0646431s</t>
+  </si>
+  <si>
+    <t>91.4790595s</t>
+  </si>
+  <si>
+    <t>187.7155729s</t>
+  </si>
+  <si>
+    <t>11.8318ms</t>
+  </si>
+  <si>
+    <t>6.8578ms</t>
+  </si>
+  <si>
+    <t>39.4984ms</t>
+  </si>
+  <si>
+    <t>43.0174ms</t>
+  </si>
+  <si>
+    <t>61.5957ms</t>
+  </si>
+  <si>
+    <t>153.6744ms</t>
+  </si>
+  <si>
+    <t>190.6344ms</t>
+  </si>
+  <si>
+    <t>268.8263ms</t>
+  </si>
+  <si>
+    <t>587.9883ms</t>
+  </si>
+  <si>
+    <t>774.0903ms</t>
+  </si>
+  <si>
+    <t>1.7459386s</t>
+  </si>
+  <si>
+    <t>2.7942599s</t>
+  </si>
+  <si>
+    <t>5.3543303s</t>
+  </si>
+  <si>
+    <t>19.6620701s</t>
+  </si>
+  <si>
+    <t>27.4125867s</t>
+  </si>
+  <si>
+    <t>51.8374964s</t>
+  </si>
+  <si>
+    <t>7.1857ms</t>
+  </si>
+  <si>
+    <t>8.9859ms</t>
+  </si>
+  <si>
+    <t>38.421ms</t>
+  </si>
+  <si>
+    <t>44.0125ms</t>
+  </si>
+  <si>
+    <t>69.0139ms</t>
+  </si>
+  <si>
+    <t>152.222ms</t>
+  </si>
+  <si>
+    <t>180.5154ms</t>
+  </si>
+  <si>
+    <t>256.7837ms</t>
+  </si>
+  <si>
+    <t>712.2776ms</t>
+  </si>
+  <si>
+    <t>856.6551ms</t>
+  </si>
+  <si>
+    <t>2.2985676s</t>
+  </si>
+  <si>
+    <t>4.1859642s</t>
+  </si>
+  <si>
+    <t>6.1847495s</t>
+  </si>
+  <si>
+    <t>19.0844562s</t>
+  </si>
+  <si>
+    <t>27.6949264s</t>
+  </si>
+  <si>
+    <t>50.2107957s</t>
+  </si>
+  <si>
+    <t>lto + codegen = 1 + native</t>
+  </si>
+  <si>
+    <t>7.1869ms</t>
+  </si>
+  <si>
+    <t>5.0112ms</t>
+  </si>
+  <si>
+    <t>37.718ms</t>
+  </si>
+  <si>
+    <t>47.0233ms</t>
+  </si>
+  <si>
+    <t>65.2536ms</t>
+  </si>
+  <si>
+    <t>148.4981ms</t>
+  </si>
+  <si>
+    <t>192.2117ms</t>
+  </si>
+  <si>
+    <t>266.613ms</t>
+  </si>
+  <si>
+    <t>580.1844ms</t>
+  </si>
+  <si>
+    <t>779.1779ms</t>
+  </si>
+  <si>
+    <t>1.69181s</t>
+  </si>
+  <si>
+    <t>3.7113947s</t>
+  </si>
+  <si>
+    <t>5.972142s</t>
+  </si>
+  <si>
+    <t>18.2536541s</t>
+  </si>
+  <si>
+    <t>26.5196328s</t>
+  </si>
+  <si>
+    <t>47.1409157s</t>
   </si>
 </sst>
 </file>
@@ -91,12 +413,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -111,9 +445,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -395,155 +734,704 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C430C4C-9943-45B4-9907-B2ED6167B133}">
+  <dimension ref="A1:L18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="9" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H6" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>40</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>55</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>60</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>65</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>70</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" t="s">
+        <v>88</v>
+      </c>
+      <c r="H16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>75</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="H17" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>80</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A13:B29"/>
+  <dimension ref="A13:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:D13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="B15" s="3"/>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>20</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
         <v>35</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="B20" s="3"/>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="B21" s="3"/>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="B23" s="3"/>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="B24" s="3"/>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
         <v>60</v>
       </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="B25" s="3"/>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
         <v>65</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="B26" s="3"/>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
         <v>70</v>
       </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="B27" s="3"/>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
         <v>75</v>
       </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="B28" s="3"/>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
         <v>80</v>
       </c>
-      <c r="B29" t="s">
-        <v>16</v>
+      <c r="B29" s="3"/>
+      <c r="C29" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A13:B13"/>
+  <mergeCells count="16">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added object initialisation to see module
</commit_message>
<xml_diff>
--- a/tests/benchmarks.xlsx
+++ b/tests/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjeer\OneDrive - Universiteit Utrecht\Desktop\Master thesis\jip\Jip\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED749EE8-921C-4A09-B156-C3445B454EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09D25A8-6C57-406B-A08D-C9546FD91542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Build configs" sheetId="2" r:id="rId1"/>
@@ -449,10 +449,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,23 +737,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C430C4C-9943-45B4-9907-B2ED6167B133}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.36328125" customWidth="1"/>
     <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" customWidth="1"/>
+    <col min="8" max="8" width="48.7265625" customWidth="1"/>
     <col min="9" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -790,10 +790,10 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -817,10 +817,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>10</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -844,10 +844,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>15</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -871,10 +871,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>20</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>4</v>
       </c>
@@ -898,10 +898,10 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>25</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="4"/>
       <c r="C7" t="s">
         <v>5</v>
       </c>
@@ -925,10 +925,10 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>30</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>6</v>
       </c>
@@ -952,10 +952,10 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>35</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>7</v>
       </c>
@@ -979,10 +979,10 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>40</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="4"/>
       <c r="C10" t="s">
         <v>8</v>
       </c>
@@ -1006,10 +1006,10 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>45</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>9</v>
       </c>
@@ -1033,10 +1033,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>50</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="4"/>
       <c r="C12" t="s">
         <v>10</v>
       </c>
@@ -1060,10 +1060,10 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>55</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="4"/>
       <c r="C13" t="s">
         <v>11</v>
       </c>
@@ -1087,10 +1087,10 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>60</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -1114,10 +1114,10 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>65</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -1141,10 +1141,10 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>70</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" t="s">
         <v>14</v>
       </c>
@@ -1168,10 +1168,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>75</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" t="s">
         <v>15</v>
       </c>
@@ -1195,10 +1195,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>80</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="4"/>
       <c r="C18" t="s">
         <v>16</v>
       </c>
@@ -1223,6 +1223,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
@@ -1234,12 +1240,6 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A13:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1271,145 +1271,145 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>5</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>20</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="C17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>25</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="4"/>
       <c r="C18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>30</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="4"/>
       <c r="C19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>35</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="4"/>
       <c r="C20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>40</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="4"/>
       <c r="C21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>45</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="4"/>
       <c r="C22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>50</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="4"/>
       <c r="C23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>55</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="4"/>
       <c r="C24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>60</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="4"/>
       <c r="C25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
+      <c r="A26" s="4">
         <v>65</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="4"/>
       <c r="C26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+      <c r="A27" s="4">
         <v>70</v>
       </c>
-      <c r="B27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+      <c r="A28" s="4">
         <v>75</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+      <c r="A29" s="4">
         <v>80</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="4"/>
       <c r="C29" t="s">
         <v>41</v>
       </c>

</xml_diff>